<commit_message>
Calendar plan v1.3 added + Assignment updated
</commit_message>
<xml_diff>
--- a/Week6. DB_UML_interfaces design/Assignment6.xlsx
+++ b/Week6. DB_UML_interfaces design/Assignment6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Внести корректировки в описание концептуальной модели БД</t>
+  </si>
+  <si>
+    <t>Рецензирования материалов другой полгруппы</t>
+  </si>
+  <si>
+    <t>Акимутин, Бидзиля</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,6 +980,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>